<commit_message>
Screen and Transition Logic Implementation
Added the ability to transition from different screens that have
different UI Element layout.  Also implemented basic transition for a
few different screens.
</commit_message>
<xml_diff>
--- a/Item List.xlsx
+++ b/Item List.xlsx
@@ -521,20 +521,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:K11"/>
+  <dimension ref="E2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,14 +549,8 @@
       <c r="I2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>1</v>
       </c>
@@ -573,14 +566,8 @@
       <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>2</v>
       </c>
@@ -596,14 +583,8 @@
       <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -619,14 +600,8 @@
       <c r="I5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>5</v>
       </c>
@@ -642,14 +617,8 @@
       <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="J6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>7</v>
       </c>
@@ -665,14 +634,8 @@
       <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>3</v>
       </c>
@@ -688,11 +651,8 @@
       <c r="I8" t="s">
         <v>36</v>
       </c>
-      <c r="J8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>6</v>
       </c>
@@ -702,24 +662,15 @@
       <c r="I9" t="s">
         <v>37</v>
       </c>
-      <c r="J9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="J10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
         <v>39</v>
-      </c>
-      <c r="J11" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -730,14 +681,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -746,7 +770,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>